<commit_message>
Mavic 2 enterprise done
</commit_message>
<xml_diff>
--- a/DJI_Mavic_2_Enterprise/DJI_Mavic_2_Enterprise.xlsx
+++ b/DJI_Mavic_2_Enterprise/DJI_Mavic_2_Enterprise.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Kuliah\S2 ITS\Semester 2\TESIS - PROPOSAL\DATASET PREPARATION\DJI_Mavic_2_Enterprise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Kuliah\S2 ITS\Semester 2\TESIS - PROPOSAL\DATASET PREPARATION\drone-timeline\DJI_Mavic_2_Enterprise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A916B8-75BB-4C51-9A77-84BDB5F5A347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639EC140-B84F-4132-8794-ACB5EEF47227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{D2B46C34-3309-4D32-8CAA-5CD61E52CD9D}"/>
   </bookViews>
@@ -1241,12 +1241,13 @@
   <dimension ref="A1:FL23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B14" sqref="B14:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:168" x14ac:dyDescent="0.25">
@@ -10394,12 +10395,13 @@
   <dimension ref="A1:FL32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B25" sqref="B25:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:168" x14ac:dyDescent="0.25">
@@ -23432,7 +23434,7 @@
   <dimension ref="A1:FL29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B21" sqref="B21:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>